<commit_message>
Add trt_description to template
</commit_message>
<xml_diff>
--- a/www/data-entry-template/GLATAR_data_entry_template_v12.xlsx
+++ b/www/data-entry-template/GLATAR_data_entry_template_v12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benhlina/Library/CloudStorage/Dropbox/GitHub/NAAEDApp/www/data-entry-template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benhlina/Library/CloudStorage/Dropbox/GitHub/GLATAR-App/www/data-entry-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901536D6-FBE3-524F-BF14-B6A72B6BBA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E7291C-688C-3646-A63C-35F361D6C4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19460" activeTab="2" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="34560" windowHeight="19460" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="tbl_samples" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_dictionary!$A$4:$D$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_dictionary!$A$4:$D$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
     <author>Ben Hlina</author>
   </authors>
   <commentList>
-    <comment ref="AK5" authorId="0" shapeId="0" xr:uid="{B4D33EEE-BEDB-B341-9363-9D1C96784118}">
+    <comment ref="AL5" authorId="0" shapeId="0" xr:uid="{B4D33EEE-BEDB-B341-9363-9D1C96784118}">
       <text>
         <r>
           <rPr>
@@ -80,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL5" authorId="0" shapeId="0" xr:uid="{238ED598-C074-2B4E-A8CF-63B7194C3AEA}">
+    <comment ref="AM5" authorId="0" shapeId="0" xr:uid="{238ED598-C074-2B4E-A8CF-63B7194C3AEA}">
       <text>
         <r>
           <rPr>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="235">
   <si>
     <t>Field Name</t>
   </si>
@@ -988,6 +988,15 @@
   </si>
   <si>
     <t>genus_species</t>
+  </si>
+  <si>
+    <t>trt_description</t>
+  </si>
+  <si>
+    <t>as in: control: format: character</t>
+  </si>
+  <si>
+    <t>For lab studies what was the treatment (e.g., control)</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1338,6 +1347,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1679,11 +1691,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDB0B4B-8041-E244-B061-95D35DE0CD3B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2163,28 +2175,28 @@
       <c r="A36" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B36" s="39" t="s">
-        <v>9</v>
+      <c r="B36" s="51" t="s">
+        <v>232</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>45</v>
+        <v>233</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>230</v>
+        <v>177</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>144</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2192,27 +2204,27 @@
         <v>230</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>222</v>
+        <v>54</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>177</v>
+        <v>230</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>137</v>
+        <v>222</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -2220,13 +2232,13 @@
         <v>177</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2234,13 +2246,13 @@
         <v>177</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -2248,27 +2260,27 @@
         <v>177</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>85</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B43" s="40" t="s">
-        <v>11</v>
+      <c r="B43" s="39" t="s">
+        <v>82</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -2276,27 +2288,27 @@
         <v>177</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="39" t="s">
-        <v>149</v>
+        <v>177</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>87</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>151</v>
+        <v>88</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>152</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -2304,13 +2316,13 @@
         <v>19</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>20</v>
+        <v>149</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>30</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2318,13 +2330,13 @@
         <v>19</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>227</v>
+        <v>59</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2332,13 +2344,13 @@
         <v>19</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>63</v>
+        <v>227</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2346,27 +2358,27 @@
         <v>19</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>205</v>
+        <v>63</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="56" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="56" x14ac:dyDescent="0.2">
@@ -2374,55 +2386,55 @@
         <v>19</v>
       </c>
       <c r="B51" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="56" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B53" s="43" t="s">
-        <v>127</v>
+      <c r="B53" s="41" t="s">
+        <v>76</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>229</v>
+        <v>78</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>141</v>
+      <c r="B54" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2430,13 +2442,13 @@
         <v>31</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2444,41 +2456,41 @@
         <v>31</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>145</v>
+        <v>209</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B57" s="44" t="s">
-        <v>135</v>
+      <c r="B57" s="39" t="s">
+        <v>178</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>219</v>
+        <v>145</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B58" s="39" t="s">
-        <v>175</v>
+      <c r="B58" s="44" t="s">
+        <v>135</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2486,27 +2498,27 @@
         <v>31</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B60" s="44" t="s">
-        <v>179</v>
+      <c r="B60" s="39" t="s">
+        <v>176</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2514,27 +2526,27 @@
         <v>31</v>
       </c>
       <c r="B61" s="44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="39" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B62" s="44" t="s">
+        <v>180</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>55</v>
+        <v>212</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>46</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2542,13 +2554,13 @@
         <v>33</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2556,13 +2568,13 @@
         <v>33</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2570,13 +2582,13 @@
         <v>33</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2584,13 +2596,13 @@
         <v>33</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2598,27 +2610,27 @@
         <v>33</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2626,13 +2638,13 @@
         <v>42</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2640,13 +2652,13 @@
         <v>42</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2654,12 +2666,26 @@
         <v>42</v>
       </c>
       <c r="B71" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2788,13 +2814,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED99CF4A-5D49-794D-A1CB-3B08F37AF445}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AZ5"/>
+  <dimension ref="A1:BA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="5" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="9" ySplit="5" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2808,26 +2834,26 @@
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="13" customWidth="1"/>
     <col min="14" max="14" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.5" customWidth="1"/>
-    <col min="30" max="30" width="10.83203125" customWidth="1"/>
-    <col min="31" max="31" width="11.5" customWidth="1"/>
-    <col min="32" max="32" width="15.33203125" customWidth="1"/>
-    <col min="33" max="33" width="17.5" customWidth="1"/>
-    <col min="34" max="34" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="46" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.5" customWidth="1"/>
+    <col min="31" max="31" width="10.83203125" customWidth="1"/>
+    <col min="32" max="32" width="11.5" customWidth="1"/>
+    <col min="33" max="33" width="15.33203125" customWidth="1"/>
+    <col min="34" max="34" width="17.5" customWidth="1"/>
+    <col min="35" max="35" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>195</v>
       </c>
@@ -2837,7 +2863,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
         <v>27</v>
       </c>
@@ -2845,7 +2871,7 @@
       <c r="C2" s="50"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" s="49"/>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -2853,24 +2879,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>177</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>19</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>31</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AR4" t="s">
         <v>33</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AX4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:52" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>17</v>
       </c>
@@ -2920,111 +2946,114 @@
         <v>16</v>
       </c>
       <c r="Q5" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="R5" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="R5" s="24" t="s">
+      <c r="S5" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="T5" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="T5" s="24" t="s">
+      <c r="U5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="24" t="s">
+      <c r="V5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="W5" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="W5" s="25" t="s">
+      <c r="X5" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="X5" s="23" t="s">
+      <c r="Y5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="26" t="s">
+      <c r="Z5" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="AA5" s="24" t="s">
+      <c r="AB5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AB5" s="24" t="s">
+      <c r="AC5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AC5" s="24" t="s">
+      <c r="AD5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AD5" s="24" t="s">
+      <c r="AE5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AE5" s="28" t="s">
+      <c r="AF5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="AF5" s="28" t="s">
+      <c r="AG5" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="AG5" s="27" t="s">
+      <c r="AH5" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="AH5" s="28" t="s">
+      <c r="AI5" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="AI5" s="24" t="s">
+      <c r="AJ5" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="AJ5" s="24" t="s">
+      <c r="AK5" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="AK5" s="24" t="s">
+      <c r="AL5" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="AL5" s="24" t="s">
+      <c r="AM5" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="AM5" s="25" t="s">
+      <c r="AN5" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="AN5" s="25" t="s">
+      <c r="AO5" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="AO5" s="25" t="s">
+      <c r="AP5" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="AP5" s="25" t="s">
+      <c r="AQ5" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="AQ5" s="24" t="s">
+      <c r="AR5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AR5" s="24" t="s">
+      <c r="AS5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="AS5" s="24" t="s">
+      <c r="AT5" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AT5" s="24" t="s">
+      <c r="AU5" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AU5" s="24" t="s">
+      <c r="AV5" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AV5" s="24" t="s">
+      <c r="AW5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AW5" s="24" t="s">
+      <c r="AX5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AX5" s="24" t="s">
+      <c r="AY5" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AY5" s="24" t="s">
+      <c r="AZ5" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AZ5" s="24" t="s">
+      <c r="BA5" s="24" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3038,7 +3067,7 @@
   </mergeCells>
   <dataValidations count="13">
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Unknown sex " error="You have entered an unknown value for sex " promptTitle="Sex" sqref="N5" xr:uid="{61B800F7-85EA-B74C-8D79-217EB2BB8728}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S6:S999" xr:uid="{C1262AB6-4400-D04A-976B-8F918C2989AD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T6:T999" xr:uid="{C1262AB6-4400-D04A-976B-8F918C2989AD}">
       <formula1>"Total, Fork, Standard, Carapace"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6:N999" xr:uid="{8B693881-68ED-E14E-BF9E-57D22ABE1721}">
@@ -3053,25 +3082,25 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P999" xr:uid="{D59253B5-564B-1D47-923E-DC586A575C35}">
       <formula1>"wild, lab"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V6:V999" xr:uid="{C755E85C-A899-4249-A46D-96F0A4790228}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W6:W999" xr:uid="{C755E85C-A899-4249-A46D-96F0A4790228}">
       <formula1>"individual, composite, mean, equation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X6:X999" xr:uid="{DE8D5097-D7B7-D64B-9AA3-BBCDB593CD44}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6:Y999" xr:uid="{DE8D5097-D7B7-D64B-9AA3-BBCDB593CD44}">
       <formula1>"muscle, liver, stomach, scales, otolith, spines, cleithra, whole body"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6:Z999" xr:uid="{618BEA16-FB85-144A-9DB4-305EFF123E53}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:AA999" xr:uid="{618BEA16-FB85-144A-9DB4-305EFF123E53}">
       <formula1>"wet, dried"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ999" xr:uid="{66E4A2BE-9678-EC4D-BD77-D6B9C6555CFA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK999" xr:uid="{66E4A2BE-9678-EC4D-BD77-D6B9C6555CFA}">
       <formula1>"wet, dry"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U6:U9999" xr:uid="{4A464527-0C39-9F4B-9AC7-BBC9D03229A6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V6:V9999" xr:uid="{4A464527-0C39-9F4B-9AC7-BBC9D03229A6}">
       <formula1>"g"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK1001:AK9999 AL6:AL1000" xr:uid="{E08CD4DA-AE11-DB40-922E-0C3ECAF74329}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL1001:AL9999 AM6:AM1000" xr:uid="{E08CD4DA-AE11-DB40-922E-0C3ECAF74329}">
       <formula1>"Joules/g"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AG1000" xr:uid="{9917EF8E-9D15-EA4E-B86B-60B39CF888A1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH1000" xr:uid="{9917EF8E-9D15-EA4E-B86B-60B39CF888A1}">
       <formula1>"Parr oxygen bomb, Parr semi-micro oxygen bomb, Phillipson microbomb, Gentry-Weigert bomb, Unknown bomb, Proximate composition, Organic analysis, Wet digestion, Unknown"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated glatar entry tmeplate
</commit_message>
<xml_diff>
--- a/www/data-entry-template/GLATAR_data_entry_template_v12.xlsx
+++ b/www/data-entry-template/GLATAR_data_entry_template_v12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benhlina/Library/CloudStorage/Dropbox/GitHub/GLATAR-App/www/data-entry-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E7291C-688C-3646-A63C-35F361D6C4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC279F39-EE2B-C342-8DFF-F1E32BFF8416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="34560" windowHeight="19460" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19460" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="234">
   <si>
     <t>Field Name</t>
   </si>
@@ -837,9 +837,6 @@
     <t>y_units</t>
   </si>
   <si>
-    <t>C:N</t>
-  </si>
-  <si>
     <t>The slope for energy density equations</t>
   </si>
   <si>
@@ -978,9 +975,6 @@
     <t>as: Point Petre; format: character</t>
   </si>
   <si>
-    <t>as in: benjamin.hlina@gmail.com - valuid email address; format: character</t>
-  </si>
-  <si>
     <t xml:space="preserve">as in: 1.35; format: numeric; places 2 decmials </t>
   </si>
   <si>
@@ -997,6 +991,9 @@
   </si>
   <si>
     <t>For lab studies what was the treatment (e.g., control)</t>
+  </si>
+  <si>
+    <t>as in: benjamin.hlina@gmail.com - valid email address; format: character</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1347,9 +1344,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1693,9 +1687,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1733,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5" s="42" t="s">
         <v>17</v>
@@ -1753,7 +1747,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" s="45" t="s">
         <v>4</v>
@@ -1773,7 +1767,7 @@
         <v>93</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>108</v>
@@ -1787,7 +1781,7 @@
         <v>94</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>109</v>
@@ -1801,7 +1795,7 @@
         <v>95</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>110</v>
@@ -1815,7 +1809,7 @@
         <v>96</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>111</v>
@@ -1829,7 +1823,7 @@
         <v>97</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>112</v>
@@ -1857,7 +1851,7 @@
         <v>98</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>115</v>
@@ -1871,10 +1865,10 @@
         <v>166</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1885,10 +1879,10 @@
         <v>167</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1938,7 +1932,7 @@
         <v>105</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>122</v>
@@ -1955,7 +1949,7 @@
         <v>103</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>124</v>
@@ -1997,7 +1991,7 @@
         <v>79</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>155</v>
@@ -2011,10 +2005,10 @@
         <v>5</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2025,7 +2019,7 @@
         <v>129</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>130</v>
@@ -2042,7 +2036,7 @@
         <v>113</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2053,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>13</v>
@@ -2064,10 +2058,10 @@
         <v>177</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>156</v>
@@ -2081,7 +2075,7 @@
         <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>153</v>
@@ -2095,7 +2089,7 @@
         <v>150</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>154</v>
@@ -2109,7 +2103,7 @@
         <v>160</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>161</v>
@@ -2137,7 +2131,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>44</v>
@@ -2151,7 +2145,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>14</v>
@@ -2175,14 +2169,14 @@
       <c r="A36" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="39" t="s">
+        <v>230</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2201,7 +2195,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B38" s="39" t="s">
         <v>131</v>
@@ -2215,13 +2209,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B39" s="39" t="s">
         <v>132</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>143</v>
@@ -2347,7 +2341,7 @@
         <v>22</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>64</v>
@@ -2375,7 +2369,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>66</v>
@@ -2389,7 +2383,7 @@
         <v>25</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>29</v>
@@ -2403,7 +2397,7 @@
         <v>26</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>159</v>
@@ -2431,7 +2425,7 @@
         <v>127</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>142</v>
@@ -2445,7 +2439,7 @@
         <v>171</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>141</v>
@@ -2459,7 +2453,7 @@
         <v>133</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>146</v>
@@ -2487,7 +2481,7 @@
         <v>135</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>148</v>
@@ -2501,10 +2495,10 @@
         <v>175</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2515,10 +2509,10 @@
         <v>176</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2529,10 +2523,10 @@
         <v>179</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2543,10 +2537,10 @@
         <v>180</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2680,13 +2674,13 @@
         <v>42</v>
       </c>
       <c r="B72" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2722,12 +2716,12 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2816,11 +2810,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BA5"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="5" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
+    <sheetView topLeftCell="G1" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6:Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2855,12 +2846,12 @@
   <sheetData>
     <row r="1" spans="1:53" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
@@ -2922,7 +2913,7 @@
         <v>91</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J5" s="24" t="s">
         <v>18</v>
@@ -2946,7 +2937,7 @@
         <v>16</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="R5" s="24" t="s">
         <v>74</v>
@@ -3054,7 +3045,7 @@
         <v>41</v>
       </c>
       <c r="BA5" s="24" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATE TEMPLATE - SPELLING/DATABASE NAMES
</commit_message>
<xml_diff>
--- a/www/data-entry-template/GLATAR_data_entry_template_v12.xlsx
+++ b/www/data-entry-template/GLATAR_data_entry_template_v12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benhlina/Library/CloudStorage/Dropbox/GitHub/GLATAR-App/www/data-entry-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC279F39-EE2B-C342-8DFF-F1E32BFF8416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B5B807-2574-3D4D-83C8-4E3C0418E839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19460" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19460" activeTab="1" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -867,18 +867,9 @@
     <t>Journal volume number</t>
   </si>
   <si>
-    <t>PLEASE SUBMIT THIS DATA SHEET BY UPLOADING IT TO THE ATLAS DATABASE. IF YOU HAVE ISSUES OR QUESTIONS PLEASE CONTACT THE DATABASE MANAGER AT: benjamin.hlina@gmail.com</t>
-  </si>
-  <si>
     <t>tbl_source;tbl_samples</t>
   </si>
   <si>
-    <t>SOURCES-TROPHIC RELATIONSHIP</t>
-  </si>
-  <si>
-    <t>SAMPLES-TROPHIC RELATIONSHIP</t>
-  </si>
-  <si>
     <t>as in: Journal Article; format: character</t>
   </si>
   <si>
@@ -994,6 +985,15 @@
   </si>
   <si>
     <t>as in: benjamin.hlina@gmail.com - valid email address; format: character</t>
+  </si>
+  <si>
+    <t>PLEASE SUBMIT THIS DATA SHEET BY UPLOADING IT TO THE GLATAR DATABASE. IF YOU HAVE ISSUES OR QUESTIONS PLEASE CONTACT THE DATABASE MANAGER AT: benjamin.hlina@gmail.com</t>
+  </si>
+  <si>
+    <t>SAMPLES-ENERGY DENSITY/TROPHIC RELATIONSHIP</t>
+  </si>
+  <si>
+    <t>SOURCES-ENERGY DENSITY/TROPHIC RELATIONSHIP</t>
   </si>
 </sst>
 </file>
@@ -1687,9 +1687,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="42" t="s">
         <v>17</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" s="45" t="s">
         <v>4</v>
@@ -1767,7 +1767,7 @@
         <v>93</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>108</v>
@@ -1781,7 +1781,7 @@
         <v>94</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>109</v>
@@ -1795,7 +1795,7 @@
         <v>95</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>110</v>
@@ -1809,7 +1809,7 @@
         <v>96</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>111</v>
@@ -1823,7 +1823,7 @@
         <v>97</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>112</v>
@@ -1851,7 +1851,7 @@
         <v>98</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>115</v>
@@ -1879,7 +1879,7 @@
         <v>167</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>189</v>
@@ -1932,7 +1932,7 @@
         <v>105</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>122</v>
@@ -1949,7 +1949,7 @@
         <v>103</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>124</v>
@@ -1991,7 +1991,7 @@
         <v>79</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>155</v>
@@ -2005,10 +2005,10 @@
         <v>5</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2019,7 +2019,7 @@
         <v>129</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>130</v>
@@ -2036,7 +2036,7 @@
         <v>113</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2047,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>13</v>
@@ -2058,10 +2058,10 @@
         <v>177</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>156</v>
@@ -2075,7 +2075,7 @@
         <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>153</v>
@@ -2089,7 +2089,7 @@
         <v>150</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>154</v>
@@ -2103,7 +2103,7 @@
         <v>160</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>161</v>
@@ -2131,7 +2131,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>44</v>
@@ -2145,7 +2145,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>14</v>
@@ -2170,13 +2170,13 @@
         <v>177</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2195,7 +2195,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B38" s="39" t="s">
         <v>131</v>
@@ -2209,13 +2209,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B39" s="39" t="s">
         <v>132</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>143</v>
@@ -2341,7 +2341,7 @@
         <v>22</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>64</v>
@@ -2369,7 +2369,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>66</v>
@@ -2383,7 +2383,7 @@
         <v>25</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>29</v>
@@ -2397,7 +2397,7 @@
         <v>26</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>159</v>
@@ -2425,7 +2425,7 @@
         <v>127</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>142</v>
@@ -2439,7 +2439,7 @@
         <v>171</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>141</v>
@@ -2453,7 +2453,7 @@
         <v>133</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>146</v>
@@ -2481,7 +2481,7 @@
         <v>135</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>148</v>
@@ -2495,7 +2495,7 @@
         <v>175</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>181</v>
@@ -2509,7 +2509,7 @@
         <v>176</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>182</v>
@@ -2523,7 +2523,7 @@
         <v>179</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>183</v>
@@ -2537,7 +2537,7 @@
         <v>180</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>184</v>
@@ -2696,11 +2696,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422A67CE-83F0-2A4B-88E8-E8A3F38049A2}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView zoomScale="159" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2716,12 +2716,12 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="29" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2810,8 +2810,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BA5"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6:Y7"/>
+    <sheetView zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="9" ySplit="5" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2846,12 +2849,12 @@
   <sheetData>
     <row r="1" spans="1:53" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="9" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
@@ -2913,7 +2916,7 @@
         <v>91</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J5" s="24" t="s">
         <v>18</v>
@@ -2937,7 +2940,7 @@
         <v>16</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="R5" s="24" t="s">
         <v>74</v>

</xml_diff>